<commit_message>
Finish V2 and Update excel
</commit_message>
<xml_diff>
--- a/challenge/House_Prices_Advanced_Regression_Techniques/Predict_House.xlsx
+++ b/challenge/House_Prices_Advanced_Regression_Techniques/Predict_House.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ML\challenge\House_Prices_Advanced_Regression_Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01314AC-6EC4-4D01-9FA8-32E1C68CCBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ACDA66-8098-4153-8BEA-894DBE578205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC850185-87C0-4159-BE0E-47F0A5872F9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -59,10 +59,22 @@
     <t>Feature</t>
   </si>
   <si>
-    <t xml:space="preserve">Loại bỏ hết các cột bị thiếu </t>
-  </si>
-  <si>
     <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
+  </si>
+  <si>
+    <t>V1_2</t>
+  </si>
+  <si>
+    <t>Xóa các cột bị thiếu</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>Xóa các cột có dữ liệu thiếu trên 50%,điền trung vị cho các cột có dữ liệu dưới 50% bị thiếu</t>
   </si>
 </sst>
 </file>
@@ -441,16 +453,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D04272-26EA-43C9-810D-DDBF6A3663A5}">
-  <dimension ref="A2:E4"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,10 +499,44 @@
         <v>0.40637000000000001</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0.61070000000000002</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0.35859999999999997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>